<commit_message>
reverse the order of U1,U2,U3 of down_mwdc. corresponding files has been generated
</commit_message>
<xml_diff>
--- a/MWDC_mapping.xlsx
+++ b/MWDC_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="467" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="430" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="up" sheetId="1" state="visible" r:id="rId2"/>
@@ -917,162 +917,162 @@
     <t>11002F</t>
   </si>
   <si>
+    <t>20009</t>
+  </si>
+  <si>
+    <t>10020</t>
+  </si>
+  <si>
+    <t>20019</t>
+  </si>
+  <si>
+    <t>20008</t>
+  </si>
+  <si>
+    <t>10021</t>
+  </si>
+  <si>
+    <t>20018</t>
+  </si>
+  <si>
+    <t>20007</t>
+  </si>
+  <si>
+    <t>10022</t>
+  </si>
+  <si>
+    <t>20017</t>
+  </si>
+  <si>
+    <t>20006</t>
+  </si>
+  <si>
+    <t>10023</t>
+  </si>
+  <si>
+    <t>20016</t>
+  </si>
+  <si>
+    <t>20005</t>
+  </si>
+  <si>
+    <t>10024</t>
+  </si>
+  <si>
+    <t>20015</t>
+  </si>
+  <si>
+    <t>120069</t>
+  </si>
+  <si>
+    <t>20004</t>
+  </si>
+  <si>
+    <t>10025</t>
+  </si>
+  <si>
+    <t>20014</t>
+  </si>
+  <si>
+    <t>120068</t>
+  </si>
+  <si>
+    <t>20003</t>
+  </si>
+  <si>
+    <t>10026</t>
+  </si>
+  <si>
+    <t>20013</t>
+  </si>
+  <si>
+    <t>120067</t>
+  </si>
+  <si>
+    <t>20002</t>
+  </si>
+  <si>
+    <t>10027</t>
+  </si>
+  <si>
+    <t>20012</t>
+  </si>
+  <si>
+    <t>120066</t>
+  </si>
+  <si>
+    <t>20001</t>
+  </si>
+  <si>
+    <t>10028</t>
+  </si>
+  <si>
+    <t>20011</t>
+  </si>
+  <si>
+    <t>120065</t>
+  </si>
+  <si>
     <t>20000</t>
   </si>
   <si>
-    <t>10020</t>
+    <t>10029</t>
+  </si>
+  <si>
+    <t>20010</t>
+  </si>
+  <si>
+    <t>120064</t>
+  </si>
+  <si>
+    <t>1002A</t>
+  </si>
+  <si>
+    <t>2000F</t>
+  </si>
+  <si>
+    <t>120063</t>
+  </si>
+  <si>
+    <t>1002B</t>
+  </si>
+  <si>
+    <t>2000E</t>
+  </si>
+  <si>
+    <t>120062</t>
+  </si>
+  <si>
+    <t>1002C</t>
+  </si>
+  <si>
+    <t>2000D</t>
+  </si>
+  <si>
+    <t>120061</t>
+  </si>
+  <si>
+    <t>1002D</t>
+  </si>
+  <si>
+    <t>2000C</t>
+  </si>
+  <si>
+    <t>120060</t>
+  </si>
+  <si>
+    <t>1002E</t>
+  </si>
+  <si>
+    <t>2000B</t>
+  </si>
+  <si>
+    <t>1002F</t>
   </si>
   <si>
     <t>2000A</t>
   </si>
   <si>
-    <t>20001</t>
-  </si>
-  <si>
-    <t>10021</t>
-  </si>
-  <si>
-    <t>2000B</t>
-  </si>
-  <si>
-    <t>20002</t>
-  </si>
-  <si>
-    <t>10022</t>
-  </si>
-  <si>
-    <t>2000C</t>
-  </si>
-  <si>
-    <t>20003</t>
-  </si>
-  <si>
-    <t>10023</t>
-  </si>
-  <si>
-    <t>2000D</t>
-  </si>
-  <si>
-    <t>20004</t>
-  </si>
-  <si>
-    <t>10024</t>
-  </si>
-  <si>
-    <t>2000E</t>
-  </si>
-  <si>
-    <t>120069</t>
-  </si>
-  <si>
-    <t>20005</t>
-  </si>
-  <si>
-    <t>10025</t>
-  </si>
-  <si>
-    <t>2000F</t>
-  </si>
-  <si>
-    <t>120068</t>
-  </si>
-  <si>
-    <t>20006</t>
-  </si>
-  <si>
-    <t>10026</t>
-  </si>
-  <si>
-    <t>20010</t>
-  </si>
-  <si>
-    <t>120067</t>
-  </si>
-  <si>
-    <t>20007</t>
-  </si>
-  <si>
-    <t>10027</t>
-  </si>
-  <si>
-    <t>20011</t>
-  </si>
-  <si>
-    <t>120066</t>
-  </si>
-  <si>
-    <t>20008</t>
-  </si>
-  <si>
-    <t>10028</t>
-  </si>
-  <si>
-    <t>20012</t>
-  </si>
-  <si>
-    <t>120065</t>
-  </si>
-  <si>
-    <t>20009</t>
-  </si>
-  <si>
-    <t>10029</t>
-  </si>
-  <si>
-    <t>20013</t>
-  </si>
-  <si>
-    <t>120064</t>
-  </si>
-  <si>
-    <t>1002A</t>
-  </si>
-  <si>
-    <t>20014</t>
-  </si>
-  <si>
-    <t>120063</t>
-  </si>
-  <si>
-    <t>1002B</t>
-  </si>
-  <si>
-    <t>20015</t>
-  </si>
-  <si>
-    <t>120062</t>
-  </si>
-  <si>
-    <t>1002C</t>
-  </si>
-  <si>
-    <t>20016</t>
-  </si>
-  <si>
-    <t>120061</t>
-  </si>
-  <si>
-    <t>1002D</t>
-  </si>
-  <si>
-    <t>20017</t>
-  </si>
-  <si>
-    <t>120060</t>
-  </si>
-  <si>
-    <t>1002E</t>
-  </si>
-  <si>
-    <t>20018</t>
-  </si>
-  <si>
-    <t>1002F</t>
-  </si>
-  <si>
-    <t>20019</t>
-  </si>
-  <si>
     <t>110040</t>
   </si>
   <si>
@@ -1265,142 +1265,142 @@
     <t>10030</t>
   </si>
   <si>
+    <t>20029</t>
+  </si>
+  <si>
+    <t>20039</t>
+  </si>
+  <si>
+    <t>20049</t>
+  </si>
+  <si>
+    <t>20028</t>
+  </si>
+  <si>
+    <t>20038</t>
+  </si>
+  <si>
+    <t>20048</t>
+  </si>
+  <si>
+    <t>20027</t>
+  </si>
+  <si>
+    <t>20037</t>
+  </si>
+  <si>
+    <t>20047</t>
+  </si>
+  <si>
+    <t>20026</t>
+  </si>
+  <si>
+    <t>20036</t>
+  </si>
+  <si>
+    <t>20046</t>
+  </si>
+  <si>
+    <t>20025</t>
+  </si>
+  <si>
+    <t>20035</t>
+  </si>
+  <si>
+    <t>20045</t>
+  </si>
+  <si>
+    <t>20024</t>
+  </si>
+  <si>
+    <t>20034</t>
+  </si>
+  <si>
+    <t>20044</t>
+  </si>
+  <si>
+    <t>20023</t>
+  </si>
+  <si>
+    <t>20033</t>
+  </si>
+  <si>
+    <t>20043</t>
+  </si>
+  <si>
+    <t>20022</t>
+  </si>
+  <si>
+    <t>20032</t>
+  </si>
+  <si>
+    <t>20042</t>
+  </si>
+  <si>
+    <t>20021</t>
+  </si>
+  <si>
+    <t>20031</t>
+  </si>
+  <si>
+    <t>20041</t>
+  </si>
+  <si>
+    <t>20020</t>
+  </si>
+  <si>
+    <t>20030</t>
+  </si>
+  <si>
+    <t>20040</t>
+  </si>
+  <si>
+    <t>2001F</t>
+  </si>
+  <si>
+    <t>2002F</t>
+  </si>
+  <si>
+    <t>2003F</t>
+  </si>
+  <si>
+    <t>2001E</t>
+  </si>
+  <si>
+    <t>2002E</t>
+  </si>
+  <si>
+    <t>2003E</t>
+  </si>
+  <si>
+    <t>2001D</t>
+  </si>
+  <si>
+    <t>2002D</t>
+  </si>
+  <si>
+    <t>2003D</t>
+  </si>
+  <si>
+    <t>2001C</t>
+  </si>
+  <si>
+    <t>2002C</t>
+  </si>
+  <si>
+    <t>2003C</t>
+  </si>
+  <si>
+    <t>2001B</t>
+  </si>
+  <si>
+    <t>2002B</t>
+  </si>
+  <si>
+    <t>2003B</t>
+  </si>
+  <si>
     <t>2001A</t>
-  </si>
-  <si>
-    <t>20039</t>
-  </si>
-  <si>
-    <t>20049</t>
-  </si>
-  <si>
-    <t>2001B</t>
-  </si>
-  <si>
-    <t>20038</t>
-  </si>
-  <si>
-    <t>20048</t>
-  </si>
-  <si>
-    <t>2001C</t>
-  </si>
-  <si>
-    <t>20037</t>
-  </si>
-  <si>
-    <t>20047</t>
-  </si>
-  <si>
-    <t>2001D</t>
-  </si>
-  <si>
-    <t>20036</t>
-  </si>
-  <si>
-    <t>20046</t>
-  </si>
-  <si>
-    <t>2001E</t>
-  </si>
-  <si>
-    <t>20035</t>
-  </si>
-  <si>
-    <t>20045</t>
-  </si>
-  <si>
-    <t>2001F</t>
-  </si>
-  <si>
-    <t>20034</t>
-  </si>
-  <si>
-    <t>20044</t>
-  </si>
-  <si>
-    <t>20020</t>
-  </si>
-  <si>
-    <t>20033</t>
-  </si>
-  <si>
-    <t>20043</t>
-  </si>
-  <si>
-    <t>20021</t>
-  </si>
-  <si>
-    <t>20032</t>
-  </si>
-  <si>
-    <t>20042</t>
-  </si>
-  <si>
-    <t>20022</t>
-  </si>
-  <si>
-    <t>20031</t>
-  </si>
-  <si>
-    <t>20041</t>
-  </si>
-  <si>
-    <t>20023</t>
-  </si>
-  <si>
-    <t>20030</t>
-  </si>
-  <si>
-    <t>20040</t>
-  </si>
-  <si>
-    <t>20024</t>
-  </si>
-  <si>
-    <t>2002F</t>
-  </si>
-  <si>
-    <t>2003F</t>
-  </si>
-  <si>
-    <t>20025</t>
-  </si>
-  <si>
-    <t>2002E</t>
-  </si>
-  <si>
-    <t>2003E</t>
-  </si>
-  <si>
-    <t>20026</t>
-  </si>
-  <si>
-    <t>2002D</t>
-  </si>
-  <si>
-    <t>2003D</t>
-  </si>
-  <si>
-    <t>20027</t>
-  </si>
-  <si>
-    <t>2002C</t>
-  </si>
-  <si>
-    <t>2003C</t>
-  </si>
-  <si>
-    <t>20028</t>
-  </si>
-  <si>
-    <t>2002B</t>
-  </si>
-  <si>
-    <t>2003B</t>
-  </si>
-  <si>
-    <t>20029</t>
   </si>
   <si>
     <t>2002A</t>
@@ -2067,7 +2067,7 @@
   <dimension ref="A1:R113"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="K143:K174 A3"/>
+      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="A108:C123 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -6908,8 +6908,8 @@
   </sheetPr>
   <dimension ref="A1:S113"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="K143:K174 A3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="P34" activeCellId="1" pane="topLeft" sqref="A108:C123 P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -7205,7 +7205,7 @@
         <v>29</v>
       </c>
       <c r="P8" s="9" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q8" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M8-1)</f>
@@ -7255,7 +7255,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="9" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M9-1)</f>
@@ -7305,7 +7305,7 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M10-1)</f>
@@ -7355,7 +7355,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q11" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M11-1)</f>
@@ -7405,7 +7405,7 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M12-1)</f>
@@ -7455,7 +7455,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M13-1)</f>
@@ -7505,7 +7505,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M14-1)</f>
@@ -7555,7 +7555,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M15-1)</f>
@@ -7605,7 +7605,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M16-1)</f>
@@ -7655,7 +7655,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="9" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M17-1)</f>
@@ -7709,7 +7709,7 @@
         <v>29</v>
       </c>
       <c r="P18" s="9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q18" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M18-1)</f>
@@ -7759,7 +7759,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="9" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q19" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M19-1)</f>
@@ -7809,7 +7809,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="9" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Q20" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M20-1)</f>
@@ -7859,7 +7859,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="9" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="Q21" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M21-1)</f>
@@ -7909,7 +7909,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="9" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q22" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M22-1)</f>
@@ -7959,7 +7959,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q23" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M23-1)</f>
@@ -8017,7 +8017,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q24" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M24-1)</f>
@@ -8067,7 +8067,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q25" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M25-1)</f>
@@ -8117,7 +8117,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q26" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M26-1)</f>
@@ -8167,7 +8167,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="Q27" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M27-1)</f>
@@ -8217,7 +8217,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q28" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M28-1)</f>
@@ -8267,7 +8267,7 @@
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="9" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q29" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M29-1)</f>
@@ -8317,7 +8317,7 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="9" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="Q30" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M30-1)</f>
@@ -8367,7 +8367,7 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="9" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="Q31" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M31-1)</f>
@@ -8417,7 +8417,7 @@
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="9" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M32-1)</f>
@@ -8467,7 +8467,7 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="9" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M33-1)</f>
@@ -8521,7 +8521,7 @@
         <v>29</v>
       </c>
       <c r="P34" s="9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q34" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M34-1)</f>
@@ -8571,7 +8571,7 @@
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="9" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q35" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M35-1)</f>
@@ -8621,7 +8621,7 @@
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="9" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Q36" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M36-1)</f>
@@ -8671,7 +8671,7 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="9" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="Q37" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M37-1)</f>
@@ -8721,7 +8721,7 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="9" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q38" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M38-1)</f>
@@ -8771,7 +8771,7 @@
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q39" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M39-1)</f>
@@ -8829,7 +8829,7 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q40" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M40-1)</f>
@@ -8879,7 +8879,7 @@
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q41" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M41-1)</f>
@@ -8929,7 +8929,7 @@
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q42" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M42-1)</f>
@@ -8979,7 +8979,7 @@
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="Q43" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M43-1)</f>
@@ -9029,7 +9029,7 @@
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q44" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M44-1)</f>
@@ -9079,7 +9079,7 @@
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="9" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q45" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M45-1)</f>
@@ -9129,7 +9129,7 @@
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
       <c r="P46" s="9" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="Q46" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M46-1)</f>
@@ -9179,7 +9179,7 @@
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="9" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="Q47" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M47-1)</f>
@@ -9229,7 +9229,7 @@
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="9" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M48-1)</f>
@@ -9279,7 +9279,7 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="9" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="9" t="n">
         <f aca="false">_xlfn.BITLSHIFT($B$2,24)+_xlfn.BITLSHIFT($D$2,20)+_xlfn.BITLSHIFT($F$4,16)+(M49-1)</f>
@@ -12062,8 +12062,8 @@
   </sheetPr>
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A139" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="K143" activeCellId="0" pane="topLeft" sqref="K143:K174"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A88" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="A108" activeCellId="0" pane="topLeft" sqref="A108:C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14744,7 +14744,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="5" t="n">
-        <v>131072</v>
+        <v>131081</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>286</v>
@@ -14764,7 +14764,7 @@
         <v>0</v>
       </c>
       <c r="N73" s="5" t="n">
-        <v>131082</v>
+        <v>131097</v>
       </c>
       <c r="O73" s="5" t="s">
         <v>288</v>
@@ -14787,7 +14787,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="5" t="n">
-        <v>131073</v>
+        <v>131080</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>289</v>
@@ -14807,7 +14807,7 @@
         <v>1</v>
       </c>
       <c r="N74" s="5" t="n">
-        <v>131083</v>
+        <v>131096</v>
       </c>
       <c r="O74" s="5" t="s">
         <v>291</v>
@@ -14830,7 +14830,7 @@
         <v>2</v>
       </c>
       <c r="F75" s="5" t="n">
-        <v>131074</v>
+        <v>131079</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>292</v>
@@ -14850,7 +14850,7 @@
         <v>2</v>
       </c>
       <c r="N75" s="5" t="n">
-        <v>131084</v>
+        <v>131095</v>
       </c>
       <c r="O75" s="5" t="s">
         <v>294</v>
@@ -14873,7 +14873,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="5" t="n">
-        <v>131075</v>
+        <v>131078</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>295</v>
@@ -14893,7 +14893,7 @@
         <v>3</v>
       </c>
       <c r="N76" s="5" t="n">
-        <v>131085</v>
+        <v>131094</v>
       </c>
       <c r="O76" s="5" t="s">
         <v>297</v>
@@ -14916,7 +14916,7 @@
         <v>4</v>
       </c>
       <c r="F77" s="5" t="n">
-        <v>131076</v>
+        <v>131077</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>298</v>
@@ -14936,7 +14936,7 @@
         <v>4</v>
       </c>
       <c r="N77" s="5" t="n">
-        <v>131086</v>
+        <v>131093</v>
       </c>
       <c r="O77" s="5" t="s">
         <v>300</v>
@@ -14957,7 +14957,7 @@
         <v>5</v>
       </c>
       <c r="F78" s="5" t="n">
-        <v>131077</v>
+        <v>131076</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>302</v>
@@ -14977,7 +14977,7 @@
         <v>5</v>
       </c>
       <c r="N78" s="5" t="n">
-        <v>131087</v>
+        <v>131092</v>
       </c>
       <c r="O78" s="5" t="s">
         <v>304</v>
@@ -14998,7 +14998,7 @@
         <v>6</v>
       </c>
       <c r="F79" s="5" t="n">
-        <v>131078</v>
+        <v>131075</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>306</v>
@@ -15018,7 +15018,7 @@
         <v>6</v>
       </c>
       <c r="N79" s="5" t="n">
-        <v>131088</v>
+        <v>131091</v>
       </c>
       <c r="O79" s="5" t="s">
         <v>308</v>
@@ -15039,7 +15039,7 @@
         <v>7</v>
       </c>
       <c r="F80" s="5" t="n">
-        <v>131079</v>
+        <v>131074</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>310</v>
@@ -15059,7 +15059,7 @@
         <v>7</v>
       </c>
       <c r="N80" s="5" t="n">
-        <v>131089</v>
+        <v>131090</v>
       </c>
       <c r="O80" s="5" t="s">
         <v>312</v>
@@ -15080,7 +15080,7 @@
         <v>8</v>
       </c>
       <c r="F81" s="5" t="n">
-        <v>131080</v>
+        <v>131073</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>314</v>
@@ -15100,7 +15100,7 @@
         <v>8</v>
       </c>
       <c r="N81" s="5" t="n">
-        <v>131090</v>
+        <v>131089</v>
       </c>
       <c r="O81" s="5" t="s">
         <v>316</v>
@@ -15121,7 +15121,7 @@
         <v>9</v>
       </c>
       <c r="F82" s="5" t="n">
-        <v>131081</v>
+        <v>131072</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>318</v>
@@ -15141,7 +15141,7 @@
         <v>9</v>
       </c>
       <c r="N82" s="5" t="n">
-        <v>131091</v>
+        <v>131088</v>
       </c>
       <c r="O82" s="5" t="s">
         <v>320</v>
@@ -15184,7 +15184,7 @@
         <v>10</v>
       </c>
       <c r="N83" s="5" t="n">
-        <v>131092</v>
+        <v>131087</v>
       </c>
       <c r="O83" s="5" t="s">
         <v>323</v>
@@ -15227,7 +15227,7 @@
         <v>11</v>
       </c>
       <c r="N84" s="5" t="n">
-        <v>131093</v>
+        <v>131086</v>
       </c>
       <c r="O84" s="5" t="s">
         <v>326</v>
@@ -15270,7 +15270,7 @@
         <v>12</v>
       </c>
       <c r="N85" s="5" t="n">
-        <v>131094</v>
+        <v>131085</v>
       </c>
       <c r="O85" s="5" t="s">
         <v>329</v>
@@ -15313,7 +15313,7 @@
         <v>13</v>
       </c>
       <c r="N86" s="5" t="n">
-        <v>131095</v>
+        <v>131084</v>
       </c>
       <c r="O86" s="5" t="s">
         <v>332</v>
@@ -15356,7 +15356,7 @@
         <v>14</v>
       </c>
       <c r="N87" s="5" t="n">
-        <v>131096</v>
+        <v>131083</v>
       </c>
       <c r="O87" s="5" t="s">
         <v>335</v>
@@ -15401,7 +15401,7 @@
         <v>15</v>
       </c>
       <c r="N88" s="5" t="n">
-        <v>131097</v>
+        <v>131082</v>
       </c>
       <c r="O88" s="5" t="s">
         <v>337</v>
@@ -16128,7 +16128,7 @@
         <v>0</v>
       </c>
       <c r="B108" s="5" t="n">
-        <v>131098</v>
+        <v>131113</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>402</v>
@@ -16171,7 +16171,7 @@
         <v>1</v>
       </c>
       <c r="B109" s="5" t="n">
-        <v>131099</v>
+        <v>131112</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>405</v>
@@ -16214,7 +16214,7 @@
         <v>2</v>
       </c>
       <c r="B110" s="5" t="n">
-        <v>131100</v>
+        <v>131111</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>408</v>
@@ -16257,7 +16257,7 @@
         <v>3</v>
       </c>
       <c r="B111" s="5" t="n">
-        <v>131101</v>
+        <v>131110</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>411</v>
@@ -16300,7 +16300,7 @@
         <v>4</v>
       </c>
       <c r="B112" s="5" t="n">
-        <v>131102</v>
+        <v>131109</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>414</v>
@@ -16343,7 +16343,7 @@
         <v>5</v>
       </c>
       <c r="B113" s="5" t="n">
-        <v>131103</v>
+        <v>131108</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>417</v>
@@ -16386,7 +16386,7 @@
         <v>6</v>
       </c>
       <c r="B114" s="5" t="n">
-        <v>131104</v>
+        <v>131107</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>420</v>
@@ -16429,7 +16429,7 @@
         <v>7</v>
       </c>
       <c r="B115" s="5" t="n">
-        <v>131105</v>
+        <v>131106</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>423</v>
@@ -16472,7 +16472,7 @@
         <v>8</v>
       </c>
       <c r="B116" s="5" t="n">
-        <v>131106</v>
+        <v>131105</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>426</v>
@@ -16515,7 +16515,7 @@
         <v>9</v>
       </c>
       <c r="B117" s="5" t="n">
-        <v>131107</v>
+        <v>131104</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>429</v>
@@ -16558,7 +16558,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="5" t="n">
-        <v>131108</v>
+        <v>131103</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>432</v>
@@ -16601,7 +16601,7 @@
         <v>11</v>
       </c>
       <c r="B119" s="5" t="n">
-        <v>131109</v>
+        <v>131102</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>435</v>
@@ -16644,7 +16644,7 @@
         <v>12</v>
       </c>
       <c r="B120" s="5" t="n">
-        <v>131110</v>
+        <v>131101</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>438</v>
@@ -16687,7 +16687,7 @@
         <v>13</v>
       </c>
       <c r="B121" s="5" t="n">
-        <v>131111</v>
+        <v>131100</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>441</v>
@@ -16730,7 +16730,7 @@
         <v>14</v>
       </c>
       <c r="B122" s="5" t="n">
-        <v>131112</v>
+        <v>131099</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>444</v>
@@ -16773,7 +16773,7 @@
         <v>15</v>
       </c>
       <c r="B123" s="5" t="n">
-        <v>131113</v>
+        <v>131098</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>447</v>
@@ -17478,16 +17478,16 @@
       </c>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
-      <c r="I141" s="9" t="s">
+      <c r="I141" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="J141" s="9"/>
-      <c r="K141" s="9"/>
-      <c r="M141" s="9" t="s">
+      <c r="J141" s="6"/>
+      <c r="K141" s="6"/>
+      <c r="M141" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="N141" s="9"/>
-      <c r="O141" s="9"/>
+      <c r="N141" s="6"/>
+      <c r="O141" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="142">
       <c r="A142" s="9" t="s">
@@ -18593,7 +18593,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="1" pane="topLeft" sqref="K143:K174 B3"/>
+      <selection activeCell="B3" activeCellId="1" pane="topLeft" sqref="A108:C123 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -18611,26 +18611,26 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="9" t="s">

</xml_diff>